<commit_message>
the fight exe is be packed but i cna't guarantee if there are any other libraries being packaged in
</commit_message>
<xml_diff>
--- a/WTF-Trans/output.xlsx
+++ b/WTF-Trans/output.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -539,7 +539,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
@@ -599,7 +599,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
@@ -659,7 +659,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
@@ -719,7 +719,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
@@ -779,7 +779,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
@@ -839,7 +839,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
@@ -899,7 +899,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
@@ -959,7 +959,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
@@ -1379,7 +1379,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
@@ -1603,7 +1603,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
@@ -1711,7 +1711,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I22" t="inlineStr"/>
@@ -1767,7 +1767,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I23" t="inlineStr"/>
@@ -1823,7 +1823,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I24" t="inlineStr"/>
@@ -1879,7 +1879,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I25" t="inlineStr"/>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I26" t="inlineStr"/>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I27" t="inlineStr"/>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I28" t="inlineStr"/>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I29" t="inlineStr"/>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I30" t="inlineStr"/>
@@ -2223,7 +2223,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I31" t="inlineStr"/>
@@ -2279,7 +2279,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I32" t="inlineStr"/>
@@ -2339,7 +2339,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I33" t="inlineStr"/>
@@ -2399,7 +2399,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I34" t="inlineStr"/>
@@ -2459,7 +2459,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I35" t="inlineStr"/>
@@ -2519,7 +2519,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I36" t="inlineStr"/>
@@ -2579,7 +2579,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I37" t="inlineStr"/>
@@ -2639,7 +2639,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I38" t="inlineStr"/>
@@ -2699,7 +2699,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I39" t="inlineStr"/>
@@ -2759,7 +2759,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I40" t="inlineStr"/>
@@ -2804,7 +2804,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2040</t>
+          <t>1040</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2819,7 +2819,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2025-05-28</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="I41" t="inlineStr"/>

</xml_diff>